<commit_message>
Save Commit - Terminando Report -
</commit_message>
<xml_diff>
--- a/Reports/Report.xlsx
+++ b/Reports/Report.xlsx
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,19 +29,22 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b val="1"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="002196F3"/>
+        <bgColor rgb="0021A6F3"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -49,21 +52,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -631,6 +626,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -896,6 +892,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -981,6 +978,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1606,6 +1604,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1871,6 +1870,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2406,6 +2406,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2761,6 +2762,7 @@
           <t>Advogado</t>
         </is>
       </c>
+      <c r="R26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3116,6 +3118,7 @@
           <t>Advogado</t>
         </is>
       </c>
+      <c r="R30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -3831,6 +3834,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3916,6 +3920,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -4721,6 +4726,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -5076,6 +5082,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -5701,6 +5708,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -6236,6 +6244,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6321,6 +6330,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -6586,6 +6596,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -6671,6 +6682,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -7206,6 +7218,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -7381,6 +7394,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -7916,6 +7930,7 @@
           <t>Advogado</t>
         </is>
       </c>
+      <c r="R84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -8631,6 +8646,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -8716,6 +8732,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -9161,6 +9178,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -9246,6 +9264,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -9691,6 +9710,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -9776,6 +9796,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -10221,6 +10242,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -10396,6 +10418,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -10481,6 +10504,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -10836,6 +10860,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -10921,6 +10946,7 @@
           <t>Advogado</t>
         </is>
       </c>
+      <c r="R118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -11906,6 +11932,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="n">
@@ -11991,6 +12018,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -12346,6 +12374,7 @@
           <t>Advogado</t>
         </is>
       </c>
+      <c r="R134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -12791,6 +12820,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -12876,6 +12906,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -13321,6 +13352,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="n">
@@ -14216,6 +14248,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -14301,6 +14334,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -14386,6 +14420,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="n">
@@ -14741,6 +14776,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -15096,6 +15132,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="n">
@@ -16351,6 +16388,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -16436,6 +16474,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -16701,6 +16740,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -16876,6 +16916,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -16961,6 +17002,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="n">
@@ -17406,6 +17448,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -17581,6 +17624,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -17936,6 +17980,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -18381,6 +18426,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -18736,6 +18782,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -19181,6 +19228,7 @@
           <t>Advogado</t>
         </is>
       </c>
+      <c r="R211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -19716,6 +19764,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="n">
@@ -19801,6 +19850,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -20156,6 +20206,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -20241,6 +20292,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -20416,6 +20468,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -20501,6 +20554,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -21036,6 +21090,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -21931,6 +21986,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -22016,6 +22072,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="n">
@@ -22101,6 +22158,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -22366,6 +22424,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -23351,6 +23410,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="n">
@@ -23436,6 +23496,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="n">
@@ -23611,6 +23672,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="n">
@@ -23876,6 +23938,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -24231,6 +24294,7 @@
           <t>Piloto</t>
         </is>
       </c>
+      <c r="R268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="n">
@@ -24496,6 +24560,7 @@
           <t>Advogado</t>
         </is>
       </c>
+      <c r="R271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="n">
@@ -24941,6 +25006,7 @@
           <t>Servidor Público</t>
         </is>
       </c>
+      <c r="R276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="n">
@@ -25026,6 +25092,7 @@
           <t>Médico</t>
         </is>
       </c>
+      <c r="R277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="n">
@@ -25561,6 +25628,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -25736,6 +25804,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="n">
@@ -26001,6 +26070,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -26446,6 +26516,7 @@
           <t>Padre</t>
         </is>
       </c>
+      <c r="R293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -26531,6 +26602,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="n">
@@ -26616,6 +26688,7 @@
           <t>Pedreiro</t>
         </is>
       </c>
+      <c r="R295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="n">
@@ -26971,6 +27044,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -27146,6 +27220,7 @@
           <t>Soldado</t>
         </is>
       </c>
+      <c r="R301" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -27327,6 +27402,14 @@
           <t>10</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>